<commit_message>
fixed admin settings and cron issue
</commit_message>
<xml_diff>
--- a/Daily-Attendance-2026-01-08.xlsx
+++ b/Daily-Attendance-2026-01-08.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>Employee Code</t>
   </si>
@@ -26,6 +26,111 @@
   </si>
   <si>
     <t>Working Hours</t>
+  </si>
+  <si>
+    <t>EMP001</t>
+  </si>
+  <si>
+    <t>Maruthi.M</t>
+  </si>
+  <si>
+    <t>02:07 am</t>
+  </si>
+  <si>
+    <t>01:00 pm</t>
+  </si>
+  <si>
+    <t>10.87</t>
+  </si>
+  <si>
+    <t>EMP575206</t>
+  </si>
+  <si>
+    <t>Bhavya</t>
+  </si>
+  <si>
+    <t>08:43 am</t>
+  </si>
+  <si>
+    <t>4.27</t>
+  </si>
+  <si>
+    <t>EMP656501</t>
+  </si>
+  <si>
+    <t>Vrushvini</t>
+  </si>
+  <si>
+    <t>09:58 am</t>
+  </si>
+  <si>
+    <t>10:21 am</t>
+  </si>
+  <si>
+    <t>0.39</t>
+  </si>
+  <si>
+    <t>EMP940311</t>
+  </si>
+  <si>
+    <t>Om Prakash</t>
+  </si>
+  <si>
+    <t>09:59 am</t>
+  </si>
+  <si>
+    <t>3.00</t>
+  </si>
+  <si>
+    <t>EMP084414</t>
+  </si>
+  <si>
+    <t>Chinmayee</t>
+  </si>
+  <si>
+    <t>10:12 am</t>
+  </si>
+  <si>
+    <t>10:13 am</t>
+  </si>
+  <si>
+    <t>0.02</t>
+  </si>
+  <si>
+    <t>EMP744311</t>
+  </si>
+  <si>
+    <t>Sneha</t>
+  </si>
+  <si>
+    <t>10:05 am</t>
+  </si>
+  <si>
+    <t>2.90</t>
+  </si>
+  <si>
+    <t>EMP025103</t>
+  </si>
+  <si>
+    <t>Karthik</t>
+  </si>
+  <si>
+    <t>10:09 am</t>
+  </si>
+  <si>
+    <t>2.84</t>
+  </si>
+  <si>
+    <t>EMP995605</t>
+  </si>
+  <si>
+    <t>Akhil</t>
+  </si>
+  <si>
+    <t>10:10 am</t>
+  </si>
+  <si>
+    <t>2.83</t>
   </si>
 </sst>
 </file>
@@ -402,13 +507,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E9"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="3" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -428,6 +533,142 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>